<commit_message>
- Added a dictionary with Ad Serving - added first few columns that create Campaign Name - added excel formula to concatenate Campaign Name
Your branch is up to date with 'origin/master'.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3351FF4-BDBB-4DDE-8CD4-6C17AE6A1148}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC6F812-8F6F-4B51-9BA8-6A869E2799FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>Device</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t>Ad 4Game</t>
+  </si>
+  <si>
+    <t>AdServingType</t>
+  </si>
+  <si>
+    <t>Click Tracker</t>
+  </si>
+  <si>
+    <t>Tracking</t>
+  </si>
+  <si>
+    <t>No Tracking</t>
   </si>
 </sst>
 </file>
@@ -430,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +457,7 @@
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -473,8 +485,11 @@
       <c r="I1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -502,8 +517,11 @@
       <c r="I2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -529,7 +547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -540,7 +558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -548,7 +566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -576,8 +594,11 @@
       <c r="I6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -605,8 +626,11 @@
       <c r="I7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>

</xml_diff>